<commit_message>
recent lab changes: 2025-05-06 15:02:20
</commit_message>
<xml_diff>
--- a/Курс 2/Основы Data Science/Лабораторные/03. Описание данных. Статистический вывод/gameandgrade.xlsx
+++ b/Курс 2/Основы Data Science/Лабораторные/03. Описание данных. Статистический вывод/gameandgrade.xlsx
@@ -5,19 +5,18 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olesteep/Documents/Study/Курс 2/Основы Data Science/Лабораторные/03. Описание данных. Статистический вывод/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olesteep/Documents/Study/Курс 2/Основы Data Science/Лабораторные/02. Структура и описание данных. Описательные характеристики/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6E5361-4C62-374D-981A-77CFA4C96FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A675A71-78D3-4344-8F3A-8637F93A7C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17080" windowHeight="21440" activeTab="2" xr2:uid="{94C2AD48-8C41-6147-84AE-58A60A9548F9}"/>
+    <workbookView xWindow="17360" yWindow="760" windowWidth="17080" windowHeight="21440" activeTab="3" xr2:uid="{94C2AD48-8C41-6147-84AE-58A60A9548F9}"/>
   </bookViews>
   <sheets>
     <sheet name="gameandgrade" sheetId="1" r:id="rId1"/>
     <sheet name="tmp" sheetId="4" r:id="rId2"/>
     <sheet name="Lab1" sheetId="3" r:id="rId3"/>
     <sheet name="Lab2" sheetId="2" r:id="rId4"/>
-    <sheet name="Lab3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gameandgrade!$A$1:$J$771</definedName>
@@ -26,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId6"/>
-    <pivotCache cacheId="18" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -66,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="71">
   <si>
     <t>Sex</t>
   </si>
@@ -263,31 +262,22 @@
     <t>низкое образование - 0, 1, 2</t>
   </si>
   <si>
-    <t>высокое образование - 3, 4, 5</t>
-  </si>
-  <si>
     <t>часто играют - 3, 4, 5</t>
   </si>
   <si>
     <t>мало играют - 0, 1, 2</t>
   </si>
   <si>
-    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (Для матери)</t>
-  </si>
-  <si>
-    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (Для отца)</t>
-  </si>
-  <si>
     <t>п</t>
   </si>
   <si>
-    <t>Названия столбцов</t>
+    <t>высокое образование - 5, 6</t>
   </si>
   <si>
-    <t>Количество по полю Playing Often</t>
+    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (для матери)</t>
   </si>
   <si>
-    <t>Таблица наблюдаемых значений</t>
+    <t>Двухвыборочный t-тест с одинаковыми дисперсиями (для отца)</t>
   </si>
 </sst>
 </file>
@@ -462,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -658,24 +648,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -875,7 +847,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -907,10 +879,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -32716,7 +32689,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74925334-BBB6-8E4D-A8C4-1418A3312DE5}" name="Сводная таблица13" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="42">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74925334-BBB6-8E4D-A8C4-1418A3312DE5}" name="Сводная таблица13" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="42">
   <location ref="B25:C33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -32834,7 +32807,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4055949-EA7B-2D47-839F-58ABF0D24DC6}" name="Сводная таблица8" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="47">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C4055949-EA7B-2D47-839F-58ABF0D24DC6}" name="Сводная таблица8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="47">
   <location ref="B51:C58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -32959,7 +32932,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20128A8E-8F8D-1F4B-B63D-08C20AED7F0D}" name="Сводная таблица12" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{20128A8E-8F8D-1F4B-B63D-08C20AED7F0D}" name="Сводная таблица12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="B101:C112" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -33084,7 +33057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B3673BB-A2E0-9945-A967-74D58F6F93D4}" name="Сводная таблица10" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="12">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B3673BB-A2E0-9945-A967-74D58F6F93D4}" name="Сводная таблица10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="12">
   <location ref="B15:C18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -33230,7 +33203,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A4080B6-CD9C-FB4D-BF75-FB8D52BE33C3}" name="Сводная таблица9" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A4080B6-CD9C-FB4D-BF75-FB8D52BE33C3}" name="Сводная таблица9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="24">
   <location ref="B77:C85" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -33350,7 +33323,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AB5542E4-160E-E945-9B5A-ED309DB05DB7}" name="Сводная таблица7" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="25">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AB5542E4-160E-E945-9B5A-ED309DB05DB7}" name="Сводная таблица7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="25">
   <location ref="B64:C70" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33471,7 +33444,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{547671A9-AF8C-FA4E-857C-C95CFB12C3D8}" name="Сводная таблица14" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="22">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{547671A9-AF8C-FA4E-857C-C95CFB12C3D8}" name="Сводная таблица14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="22">
   <location ref="B90:C97" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0">
@@ -33594,7 +33567,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E7D066-6BCD-C74A-A456-629E58FD8256}" name="Сводная таблица11" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="23">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{96E7D066-6BCD-C74A-A456-629E58FD8256}" name="Сводная таблица11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0" chartFormat="23">
   <location ref="B38:C46" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -33699,130 +33672,6 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B78405C4-E8C5-0F48-9014-1A8C505FB32C}" name="Сводная таблица1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:H17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item h="1" x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="8">
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="3"/>
-        <item h="1" x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Количество по полю Playing Often" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -34138,8 +33987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30EAD57-2722-2640-9045-129DE337E71B}">
   <dimension ref="A1:U773"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="J415" sqref="A1:J415"/>
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:J771"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -58862,8 +58711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75069B8F-3AE3-DD4F-B9E5-3A5847B7AA82}">
   <dimension ref="A1:J357"/>
   <sheetViews>
-    <sheetView topLeftCell="A291" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="A313" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -70306,7 +70155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A424681-3FE9-694E-A0B1-02F687C4B387}">
   <dimension ref="B2:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" zoomScale="142" workbookViewId="0">
+    <sheetView topLeftCell="B21" zoomScale="125" workbookViewId="0">
       <selection activeCell="C108" sqref="C102:C108"/>
     </sheetView>
   </sheetViews>
@@ -71014,8 +70863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AF8D23-ABA4-1A44-B54C-CBEFB7E9A58E}">
   <dimension ref="A2:O772"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="111" zoomScaleNormal="134" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -71043,16 +70892,16 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O4" s="17"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O5" s="17"/>
     </row>
@@ -71061,7 +70910,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O7" s="17"/>
     </row>
@@ -71069,122 +70918,129 @@
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="23" t="s">
         <v>43</v>
       </c>
       <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B10">
-        <v>1.8160919540229885</v>
-      </c>
-      <c r="C10">
-        <v>3.9516728624535316</v>
+      <c r="B10" s="21">
+        <v>71.281954022988501</v>
+      </c>
+      <c r="C10" s="21">
+        <v>87.568181818181813</v>
       </c>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B11">
-        <v>0.15183106121357898</v>
-      </c>
-      <c r="C11">
-        <v>0.73273040004438816</v>
+      <c r="B11" s="21">
+        <v>254.01051823041999</v>
+      </c>
+      <c r="C11" s="21">
+        <v>275.52989510489505</v>
       </c>
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="21">
         <v>87</v>
       </c>
-      <c r="C12">
-        <v>269</v>
+      <c r="C12" s="21">
+        <v>66</v>
       </c>
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B13">
-        <v>0.59160796179735542</v>
-      </c>
+      <c r="B13" s="21">
+        <v>263.27382615651851</v>
+      </c>
+      <c r="C13" s="21"/>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
+      <c r="B14" s="21">
+        <v>0</v>
+      </c>
+      <c r="C14" s="21"/>
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B15">
-        <v>354</v>
-      </c>
+      <c r="B15" s="21">
+        <v>151</v>
+      </c>
+      <c r="C15" s="21"/>
       <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B16">
-        <v>-22.511777725256401</v>
-      </c>
+      <c r="B16" s="21">
+        <v>-6.1489723632650639</v>
+      </c>
+      <c r="C16" s="21"/>
       <c r="O16" s="17"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B17">
-        <v>1.3738570005292101E-70</v>
-      </c>
+      <c r="B17" s="21">
+        <v>3.327541620635482E-9</v>
+      </c>
+      <c r="C17" s="21"/>
       <c r="O17" s="17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B18">
-        <v>1.6491694147322193</v>
-      </c>
+      <c r="B18" s="21">
+        <v>1.6550073865802402</v>
+      </c>
+      <c r="C18" s="21"/>
       <c r="O18" s="17"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B19">
-        <v>2.7477140010584202E-70</v>
-      </c>
+      <c r="B19" s="21">
+        <v>6.6550832412709639E-9</v>
+      </c>
+      <c r="C19" s="21"/>
       <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="13">
-        <v>1.9666878964647558</v>
-      </c>
-      <c r="C20" s="13"/>
+      <c r="B20" s="22">
+        <v>1.9757989238179368</v>
+      </c>
+      <c r="C20" s="22"/>
       <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -71194,7 +71050,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O22" s="17"/>
     </row>
@@ -71202,125 +71058,132 @@
       <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="23" t="s">
         <v>43</v>
       </c>
       <c r="O24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B25">
-        <v>1.8955223880597014</v>
-      </c>
-      <c r="C25">
-        <v>4.1141868512110724</v>
+      <c r="B25" s="21">
+        <v>72.546716417910446</v>
+      </c>
+      <c r="C25" s="21">
+        <v>84.955555555555549</v>
       </c>
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B26">
-        <v>0.15558570782451397</v>
-      </c>
-      <c r="C26">
-        <v>0.81677720107650964</v>
+      <c r="B26" s="21">
+        <v>263.24067693351412</v>
+      </c>
+      <c r="C26" s="21">
+        <v>275.37440699126097</v>
       </c>
       <c r="O26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="21">
         <v>67</v>
       </c>
-      <c r="C27">
-        <v>289</v>
+      <c r="C27" s="21">
+        <v>90</v>
       </c>
       <c r="O27" s="17"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B28">
-        <v>0.69350421080918834</v>
-      </c>
+      <c r="B28" s="21">
+        <v>270.20778645054293</v>
+      </c>
+      <c r="C28" s="21"/>
       <c r="O28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
+      <c r="B29" s="21">
+        <v>0</v>
+      </c>
+      <c r="C29" s="21"/>
       <c r="O29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B30">
-        <v>354</v>
-      </c>
+      <c r="B30" s="21">
+        <v>155</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="O30" s="17"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B31">
-        <v>-19.648454694398335</v>
-      </c>
+      <c r="B31" s="21">
+        <v>-4.6783321738193848</v>
+      </c>
+      <c r="C31" s="21"/>
       <c r="O31" s="17"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B32">
-        <v>6.0178623308766174E-59</v>
-      </c>
+      <c r="B32" s="21">
+        <v>3.1284861316859455E-6</v>
+      </c>
+      <c r="C32" s="21"/>
       <c r="O32" s="17"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B33">
-        <v>1.6491694147322193</v>
-      </c>
+      <c r="B33" s="21">
+        <v>1.6547437739197817</v>
+      </c>
+      <c r="C33" s="21"/>
       <c r="O33" s="17"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B34">
-        <v>1.2035724661753235E-58</v>
-      </c>
+      <c r="B34" s="21">
+        <v>6.2569722633718909E-6</v>
+      </c>
+      <c r="C34" s="21"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
       <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="13">
-        <v>1.9666878964647558</v>
-      </c>
-      <c r="C35" s="13"/>
+      <c r="B35" s="22">
+        <v>1.9753871310551163</v>
+      </c>
+      <c r="C35" s="22"/>
       <c r="O35" s="17"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -71526,7 +71389,7 @@
         <v>2.422857142857143</v>
       </c>
       <c r="D63" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="O63" s="17"/>
     </row>
@@ -73825,962 +73688,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2554F2A9-8B67-FE48-83C7-909D85A19072}">
-  <dimension ref="A2:H51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="22">
-        <v>26</v>
-      </c>
-      <c r="C6" s="22">
-        <v>17</v>
-      </c>
-      <c r="D6" s="22">
-        <v>16</v>
-      </c>
-      <c r="E6" s="22">
-        <v>14</v>
-      </c>
-      <c r="F6" s="22">
-        <v>18</v>
-      </c>
-      <c r="G6" s="22">
-        <v>21</v>
-      </c>
-      <c r="H6" s="22">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>2</v>
-      </c>
-      <c r="B7" s="22">
-        <v>12</v>
-      </c>
-      <c r="C7" s="22">
-        <v>18</v>
-      </c>
-      <c r="D7" s="22">
-        <v>12</v>
-      </c>
-      <c r="E7" s="22">
-        <v>23</v>
-      </c>
-      <c r="F7" s="22">
-        <v>15</v>
-      </c>
-      <c r="G7" s="22">
-        <v>26</v>
-      </c>
-      <c r="H7" s="22">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>3</v>
-      </c>
-      <c r="B8" s="22">
-        <v>27</v>
-      </c>
-      <c r="C8" s="22">
-        <v>4</v>
-      </c>
-      <c r="D8" s="22">
-        <v>7</v>
-      </c>
-      <c r="E8" s="22">
-        <v>13</v>
-      </c>
-      <c r="F8" s="22">
-        <v>6</v>
-      </c>
-      <c r="G8" s="22">
-        <v>9</v>
-      </c>
-      <c r="H8" s="22">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>4</v>
-      </c>
-      <c r="B9" s="22">
-        <v>38</v>
-      </c>
-      <c r="C9" s="22">
-        <v>30</v>
-      </c>
-      <c r="D9" s="22">
-        <v>11</v>
-      </c>
-      <c r="E9" s="22">
-        <v>23</v>
-      </c>
-      <c r="F9" s="22">
-        <v>11</v>
-      </c>
-      <c r="G9" s="22">
-        <v>35</v>
-      </c>
-      <c r="H9" s="22">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>5</v>
-      </c>
-      <c r="B10" s="22">
-        <v>8</v>
-      </c>
-      <c r="C10" s="22">
-        <v>5</v>
-      </c>
-      <c r="D10" s="22">
-        <v>3</v>
-      </c>
-      <c r="E10" s="22">
-        <v>6</v>
-      </c>
-      <c r="F10" s="22">
-        <v>6</v>
-      </c>
-      <c r="G10" s="22">
-        <v>6</v>
-      </c>
-      <c r="H10" s="22">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>6</v>
-      </c>
-      <c r="B11" s="22">
-        <v>5</v>
-      </c>
-      <c r="C11" s="22">
-        <v>3</v>
-      </c>
-      <c r="D11" s="22">
-        <v>2</v>
-      </c>
-      <c r="E11" s="22">
-        <v>2</v>
-      </c>
-      <c r="F11" s="22">
-        <v>1</v>
-      </c>
-      <c r="G11" s="22">
-        <v>8</v>
-      </c>
-      <c r="H11" s="22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>7</v>
-      </c>
-      <c r="B12" s="22">
-        <v>15</v>
-      </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22">
-        <v>7</v>
-      </c>
-      <c r="E12" s="22">
-        <v>3</v>
-      </c>
-      <c r="F12" s="22">
-        <v>5</v>
-      </c>
-      <c r="G12" s="22">
-        <v>11</v>
-      </c>
-      <c r="H12" s="22">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>8</v>
-      </c>
-      <c r="B13" s="22">
-        <v>56</v>
-      </c>
-      <c r="C13" s="22">
-        <v>23</v>
-      </c>
-      <c r="D13" s="22">
-        <v>10</v>
-      </c>
-      <c r="E13" s="22">
-        <v>17</v>
-      </c>
-      <c r="F13" s="22">
-        <v>16</v>
-      </c>
-      <c r="G13" s="22">
-        <v>18</v>
-      </c>
-      <c r="H13" s="22">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>9</v>
-      </c>
-      <c r="B14" s="22">
-        <v>25</v>
-      </c>
-      <c r="C14" s="22">
-        <v>5</v>
-      </c>
-      <c r="D14" s="22">
-        <v>2</v>
-      </c>
-      <c r="E14" s="22">
-        <v>2</v>
-      </c>
-      <c r="F14" s="22">
-        <v>5</v>
-      </c>
-      <c r="G14" s="22">
-        <v>11</v>
-      </c>
-      <c r="H14" s="22">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>10</v>
-      </c>
-      <c r="B15" s="22">
-        <v>13</v>
-      </c>
-      <c r="C15" s="22">
-        <v>1</v>
-      </c>
-      <c r="D15" s="22">
-        <v>2</v>
-      </c>
-      <c r="E15" s="22">
-        <v>6</v>
-      </c>
-      <c r="F15" s="22">
-        <v>3</v>
-      </c>
-      <c r="G15" s="22">
-        <v>7</v>
-      </c>
-      <c r="H15" s="22">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>11</v>
-      </c>
-      <c r="B16" s="22">
-        <v>2</v>
-      </c>
-      <c r="C16" s="22">
-        <v>9</v>
-      </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22">
-        <v>3</v>
-      </c>
-      <c r="F16" s="22">
-        <v>2</v>
-      </c>
-      <c r="G16" s="22">
-        <v>4</v>
-      </c>
-      <c r="H16" s="22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="22">
-        <v>227</v>
-      </c>
-      <c r="C17" s="22">
-        <v>115</v>
-      </c>
-      <c r="D17" s="22">
-        <v>72</v>
-      </c>
-      <c r="E17" s="22">
-        <v>112</v>
-      </c>
-      <c r="F17" s="22">
-        <v>88</v>
-      </c>
-      <c r="G17" s="22">
-        <v>156</v>
-      </c>
-      <c r="H17" s="22">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="23">
-        <v>0</v>
-      </c>
-      <c r="C22" s="23">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23">
-        <v>2</v>
-      </c>
-      <c r="E22" s="23">
-        <v>3</v>
-      </c>
-      <c r="F22" s="23">
-        <v>4</v>
-      </c>
-      <c r="G22" s="23">
-        <v>5</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <f>($H23*B$34)/$H$34</f>
-        <v>33.018181818181816</v>
-      </c>
-      <c r="C23">
-        <f>($H23*C$34)/$H$34</f>
-        <v>16.727272727272727</v>
-      </c>
-      <c r="D23">
-        <f>($H23*D$34)/$H$34</f>
-        <v>10.472727272727273</v>
-      </c>
-      <c r="E23">
-        <f>($H23*E$34)/$H$34</f>
-        <v>16.290909090909089</v>
-      </c>
-      <c r="F23">
-        <f>($H23*F$34)/$H$34</f>
-        <v>12.8</v>
-      </c>
-      <c r="G23">
-        <f>($H23*G$34)/$H$34</f>
-        <v>22.690909090909091</v>
-      </c>
-      <c r="H23">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <f>($H24*B$34)/$H$34</f>
-        <v>31.249350649350649</v>
-      </c>
-      <c r="C24">
-        <f>($H24*C$34)/$H$34</f>
-        <v>15.831168831168831</v>
-      </c>
-      <c r="D24">
-        <f>($H24*D$34)/$H$34</f>
-        <v>9.9116883116883123</v>
-      </c>
-      <c r="E24">
-        <f>($H24*E$34)/$H$34</f>
-        <v>15.418181818181818</v>
-      </c>
-      <c r="F24">
-        <f>($H24*F$34)/$H$34</f>
-        <v>12.114285714285714</v>
-      </c>
-      <c r="G24">
-        <f>($H24*G$34)/$H$34</f>
-        <v>21.475324675324675</v>
-      </c>
-      <c r="H24">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <f>($H25*B$34)/$H$34</f>
-        <v>19.457142857142856</v>
-      </c>
-      <c r="C25">
-        <f>($H25*C$34)/$H$34</f>
-        <v>9.8571428571428577</v>
-      </c>
-      <c r="D25">
-        <f>($H25*D$34)/$H$34</f>
-        <v>6.1714285714285717</v>
-      </c>
-      <c r="E25">
-        <f>($H25*E$34)/$H$34</f>
-        <v>9.6</v>
-      </c>
-      <c r="F25">
-        <f>($H25*F$34)/$H$34</f>
-        <v>7.5428571428571427</v>
-      </c>
-      <c r="G25">
-        <f>($H25*G$34)/$H$34</f>
-        <v>13.371428571428572</v>
-      </c>
-      <c r="H25">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f>($H26*B$34)/$H$34</f>
-        <v>43.631168831168829</v>
-      </c>
-      <c r="C26">
-        <f>($H26*C$34)/$H$34</f>
-        <v>22.103896103896105</v>
-      </c>
-      <c r="D26">
-        <f>($H26*D$34)/$H$34</f>
-        <v>13.838961038961038</v>
-      </c>
-      <c r="E26">
-        <f>($H26*E$34)/$H$34</f>
-        <v>21.527272727272727</v>
-      </c>
-      <c r="F26">
-        <f>($H26*F$34)/$H$34</f>
-        <v>16.914285714285715</v>
-      </c>
-      <c r="G26">
-        <f>($H26*G$34)/$H$34</f>
-        <v>29.984415584415583</v>
-      </c>
-      <c r="H26">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27">
-        <f>($H27*B$34)/$H$34</f>
-        <v>10.023376623376624</v>
-      </c>
-      <c r="C27">
-        <f>($H27*C$34)/$H$34</f>
-        <v>5.0779220779220777</v>
-      </c>
-      <c r="D27">
-        <f>($H27*D$34)/$H$34</f>
-        <v>3.1792207792207794</v>
-      </c>
-      <c r="E27">
-        <f>($H27*E$34)/$H$34</f>
-        <v>4.9454545454545453</v>
-      </c>
-      <c r="F27">
-        <f>($H27*F$34)/$H$34</f>
-        <v>3.8857142857142857</v>
-      </c>
-      <c r="G27">
-        <f>($H27*G$34)/$H$34</f>
-        <v>6.8883116883116884</v>
-      </c>
-      <c r="H27">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28">
-        <f>($H28*B$34)/$H$34</f>
-        <v>6.1909090909090905</v>
-      </c>
-      <c r="C28">
-        <f>($H28*C$34)/$H$34</f>
-        <v>3.1363636363636362</v>
-      </c>
-      <c r="D28">
-        <f>($H28*D$34)/$H$34</f>
-        <v>1.9636363636363636</v>
-      </c>
-      <c r="E28">
-        <f>($H28*E$34)/$H$34</f>
-        <v>3.0545454545454547</v>
-      </c>
-      <c r="F28">
-        <f>($H28*F$34)/$H$34</f>
-        <v>2.4</v>
-      </c>
-      <c r="G28">
-        <f>($H28*G$34)/$H$34</f>
-        <v>4.2545454545454549</v>
-      </c>
-      <c r="H28">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29">
-        <f>($H29*B$34)/$H$34</f>
-        <v>12.087012987012987</v>
-      </c>
-      <c r="C29">
-        <f>($H29*C$34)/$H$34</f>
-        <v>6.1233766233766236</v>
-      </c>
-      <c r="D29">
-        <f>($H29*D$34)/$H$34</f>
-        <v>3.8337662337662337</v>
-      </c>
-      <c r="E29">
-        <f>($H29*E$34)/$H$34</f>
-        <v>5.9636363636363638</v>
-      </c>
-      <c r="F29">
-        <f>($H29*F$34)/$H$34</f>
-        <v>4.6857142857142859</v>
-      </c>
-      <c r="G29">
-        <f>($H29*G$34)/$H$34</f>
-        <v>8.3064935064935064</v>
-      </c>
-      <c r="H29">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>8</v>
-      </c>
-      <c r="B30">
-        <f>($H30*B$34)/$H$34</f>
-        <v>41.272727272727273</v>
-      </c>
-      <c r="C30">
-        <f>($H30*C$34)/$H$34</f>
-        <v>20.90909090909091</v>
-      </c>
-      <c r="D30">
-        <f>($H30*D$34)/$H$34</f>
-        <v>13.090909090909092</v>
-      </c>
-      <c r="E30">
-        <f>($H30*E$34)/$H$34</f>
-        <v>20.363636363636363</v>
-      </c>
-      <c r="F30">
-        <f>($H30*F$34)/$H$34</f>
-        <v>16</v>
-      </c>
-      <c r="G30">
-        <f>($H30*G$34)/$H$34</f>
-        <v>28.363636363636363</v>
-      </c>
-      <c r="H30">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>9</v>
-      </c>
-      <c r="B31">
-        <f>($H31*B$34)/$H$34</f>
-        <v>14.74025974025974</v>
-      </c>
-      <c r="C31">
-        <f>($H31*C$34)/$H$34</f>
-        <v>7.4675324675324672</v>
-      </c>
-      <c r="D31">
-        <f>($H31*D$34)/$H$34</f>
-        <v>4.6753246753246751</v>
-      </c>
-      <c r="E31">
-        <f>($H31*E$34)/$H$34</f>
-        <v>7.2727272727272725</v>
-      </c>
-      <c r="F31">
-        <f>($H31*F$34)/$H$34</f>
-        <v>5.7142857142857144</v>
-      </c>
-      <c r="G31">
-        <f>($H31*G$34)/$H$34</f>
-        <v>10.129870129870129</v>
-      </c>
-      <c r="H31">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>10</v>
-      </c>
-      <c r="B32">
-        <f>($H32*B$34)/$H$34</f>
-        <v>9.4337662337662334</v>
-      </c>
-      <c r="C32">
-        <f>($H32*C$34)/$H$34</f>
-        <v>4.779220779220779</v>
-      </c>
-      <c r="D32">
-        <f>($H32*D$34)/$H$34</f>
-        <v>2.9922077922077923</v>
-      </c>
-      <c r="E32">
-        <f>($H32*E$34)/$H$34</f>
-        <v>4.6545454545454543</v>
-      </c>
-      <c r="F32">
-        <f>($H32*F$34)/$H$34</f>
-        <v>3.657142857142857</v>
-      </c>
-      <c r="G32">
-        <f>($H32*G$34)/$H$34</f>
-        <v>6.4831168831168835</v>
-      </c>
-      <c r="H32">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33">
-        <f>($H33*B$34)/$H$34</f>
-        <v>5.8961038961038961</v>
-      </c>
-      <c r="C33">
-        <f>($H33*C$34)/$H$34</f>
-        <v>2.9870129870129869</v>
-      </c>
-      <c r="D33">
-        <f>($H33*D$34)/$H$34</f>
-        <v>1.8701298701298701</v>
-      </c>
-      <c r="E33">
-        <f>($H33*E$34)/$H$34</f>
-        <v>2.9090909090909092</v>
-      </c>
-      <c r="F33">
-        <f>($H33*F$34)/$H$34</f>
-        <v>2.2857142857142856</v>
-      </c>
-      <c r="G33">
-        <f>($H33*G$34)/$H$34</f>
-        <v>4.0519480519480515</v>
-      </c>
-      <c r="H33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="23">
-        <v>227</v>
-      </c>
-      <c r="C34" s="23">
-        <v>115</v>
-      </c>
-      <c r="D34" s="23">
-        <v>72</v>
-      </c>
-      <c r="E34" s="23">
-        <v>112</v>
-      </c>
-      <c r="F34" s="23">
-        <v>88</v>
-      </c>
-      <c r="G34" s="23">
-        <v>156</v>
-      </c>
-      <c r="H34" s="23">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="24">
-        <v>0</v>
-      </c>
-      <c r="C39" s="24">
-        <v>1</v>
-      </c>
-      <c r="D39" s="24">
-        <v>2</v>
-      </c>
-      <c r="E39" s="24">
-        <v>3</v>
-      </c>
-      <c r="F39" s="24">
-        <v>4</v>
-      </c>
-      <c r="G39" s="24">
-        <v>5</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="e">
-        <f>((B6-B23)^2)/C18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H40">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="H41">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="H42">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="H43">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>5</v>
-      </c>
-      <c r="H44">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>6</v>
-      </c>
-      <c r="H45">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>7</v>
-      </c>
-      <c r="H46">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>8</v>
-      </c>
-      <c r="H47">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>9</v>
-      </c>
-      <c r="H48">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>10</v>
-      </c>
-      <c r="H49">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>11</v>
-      </c>
-      <c r="H50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B51" s="24">
-        <v>227</v>
-      </c>
-      <c r="C51" s="24">
-        <v>115</v>
-      </c>
-      <c r="D51" s="24">
-        <v>72</v>
-      </c>
-      <c r="E51" s="24">
-        <v>112</v>
-      </c>
-      <c r="F51" s="24">
-        <v>88</v>
-      </c>
-      <c r="G51" s="24">
-        <v>156</v>
-      </c>
-      <c r="H51" s="24">
-        <v>770</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>